<commit_message>
segment by task run on all subjects
</commit_message>
<xml_diff>
--- a/HR_Data/tmp_LWP2_0011_FirstBeat_RR_raw_data_by_task.xlsx
+++ b/HR_Data/tmp_LWP2_0011_FirstBeat_RR_raw_data_by_task.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophie\Documents\MATLAB\HeartRate\HR_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\MATLAB\Sophie_HeartRate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="10395" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10665" firstSheet="14" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>